<commit_message>
complete DRL secondary control under fixed disturbance
</commit_message>
<xml_diff>
--- a/andes_gym/envs/ieee14_alter_pq.xlsx
+++ b/andes_gym/envs/ieee14_alter_pq.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/ieee14/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yichenzhang/GitHub/andes_gym/andes_gym/envs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E2B48C-0720-2E4A-B236-5AED4F2AEF6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2088E1-1FFB-244C-AACA-C8CC2C8F10DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9640" yWindow="2920" windowWidth="25220" windowHeight="14820" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2305,7 +2305,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2389,7 +2389,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <v>-0.1</v>

</xml_diff>

<commit_message>
test with a larger disturbance
</commit_message>
<xml_diff>
--- a/andes_gym/envs/ieee14_alter_pq.xlsx
+++ b/andes_gym/envs/ieee14_alter_pq.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yichenzhang/GitHub/andes_gym/andes_gym/envs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2088E1-1FFB-244C-AACA-C8CC2C8F10DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86AE91A-0022-444E-84C6-453D1019469B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9640" yWindow="2920" windowWidth="25220" windowHeight="14820" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9640" yWindow="2920" windowWidth="25220" windowHeight="14820" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="2" r:id="rId1"/>
@@ -2303,7 +2303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
     </sheetView>
@@ -5400,9 +5400,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5474,10 +5474,10 @@
         <v>0.05</v>
       </c>
       <c r="I2">
-        <v>1.05</v>
+        <v>3</v>
       </c>
       <c r="J2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <v>0.05</v>
@@ -5515,7 +5515,7 @@
         <v>0.05</v>
       </c>
       <c r="I3">
-        <v>1.2</v>
+        <v>3</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -5556,7 +5556,7 @@
         <v>0.05</v>
       </c>
       <c r="I4">
-        <v>1.2</v>
+        <v>3</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -5597,10 +5597,10 @@
         <v>0.05</v>
       </c>
       <c r="I5">
-        <v>1.05</v>
+        <v>3</v>
       </c>
       <c r="J5">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <v>0.05</v>
@@ -5638,10 +5638,10 @@
         <v>0.05</v>
       </c>
       <c r="I6">
-        <v>1.05</v>
+        <v>3</v>
       </c>
       <c r="J6">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <v>0.05</v>

</xml_diff>